<commit_message>
realizando la implementacion de ETL para subir usuarios desde un archivo xlsx a BD
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a9db2649279a473/TelentoTech-CRUD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD87ABEE-8C72-4CF2-8DC5-86414C5E35DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{CD87ABEE-8C72-4CF2-8DC5-86414C5E35DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFDC0D08-C497-46FC-A846-14F53DA272C9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F4D82461-0FDD-4C9D-A9FA-9C8B7ED61324}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="137">
   <si>
     <t xml:space="preserve"> id </t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">  lastname  </t>
   </si>
   <si>
-    <t xml:space="preserve">             email             </t>
-  </si>
-  <si>
     <t xml:space="preserve">  password  </t>
   </si>
   <si>
@@ -63,18 +60,6 @@
     <t>------------</t>
   </si>
   <si>
-    <t xml:space="preserve">      John      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Doe     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   johndoe@example.com         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  password1 </t>
-  </si>
-  <si>
     <t xml:space="preserve">      Jane      </t>
   </si>
   <si>
@@ -426,12 +411,6 @@
     <t xml:space="preserve">  password39</t>
   </si>
   <si>
-    <t xml:space="preserve">   emmaharris@example.com             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  password40</t>
-  </si>
-  <si>
     <t xml:space="preserve">   ethanwilso11n@example.com            </t>
   </si>
   <si>
@@ -442,16 +421,59 @@
   </si>
   <si>
     <t xml:space="preserve">   jacksonw75hite@example.com           </t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>JHON</t>
+  </si>
+  <si>
+    <t>1johndoe11@example.com</t>
+  </si>
+  <si>
+    <t>DARION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,16 +496,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -824,10 +860,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7960818-CA3D-443B-B753-F9F11DE6B97E}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F32" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D2 D41:D1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BC115526-7F4F-4F01-9F28-A16B17CF9004}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBACFF8-9C9D-41EF-AAA0-DD45A48ABDCC}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,27 +947,27 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -871,16 +975,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -888,16 +992,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -905,16 +1009,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -922,16 +1026,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -939,16 +1043,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -956,16 +1060,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -973,16 +1077,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -990,16 +1094,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1007,16 +1111,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1024,16 +1128,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1041,16 +1145,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1058,16 +1162,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1075,16 +1179,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1092,16 +1196,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1109,16 +1213,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1126,16 +1230,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1143,16 +1247,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1160,16 +1264,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1177,16 +1281,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1194,16 +1298,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1211,16 +1315,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1228,16 +1332,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1245,16 +1349,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1262,16 +1366,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1279,16 +1383,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1296,16 +1400,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1313,16 +1417,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1330,16 +1434,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1347,16 +1451,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1364,16 +1468,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1381,16 +1485,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1398,16 +1502,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1415,16 +1519,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,16 +1536,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E36" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1449,16 +1553,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1466,16 +1570,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E38" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1483,16 +1587,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E39" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1500,598 +1604,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E40" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D3:D40">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBACFF8-9C9D-41EF-AAA0-DD45A48ABDCC}">
-  <dimension ref="A1:E32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>31</v>
-      </c>
-      <c r="B23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>32</v>
-      </c>
-      <c r="B24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>116</v>
-      </c>
-      <c r="E26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>38</v>
-      </c>
-      <c r="B30" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>